<commit_message>
added log returns for bonds
</commit_message>
<xml_diff>
--- a/HW3/hw4_data.xlsx
+++ b/HW3/hw4_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benclayman/Documents/benjamin-clayman-533/HW3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CB9AE8-46F1-134D-A04D-FD1EE72C00A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0C0E16-DDF1-9346-BB12-FCB5068CD73C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="26660" windowHeight="15320" xr2:uid="{5FA674BD-3039-4104-9824-F509DF8E3938}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="26660" windowHeight="15320" activeTab="1" xr2:uid="{5FA674BD-3039-4104-9824-F509DF8E3938}"/>
   </bookViews>
   <sheets>
     <sheet name="PRICES_DATA" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -422,7 +433,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14E47AB-7038-4841-85F8-7E9992289228}">
   <dimension ref="A1:K858"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -30469,8 +30482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45ACD470-24A8-4C4E-AB32-43764D3ACD3B}">
   <dimension ref="A1:C826"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>